<commit_message>
refactoring, dropping earlier versions of files
</commit_message>
<xml_diff>
--- a/model/features_testing_metrics.xlsx
+++ b/model/features_testing_metrics.xlsx
@@ -493,16 +493,16 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4560487599831862</v>
+        <v>0.4795503813729426</v>
       </c>
       <c r="G2" t="n">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4534253246753246</v>
+        <v>0.4795833333333333</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -526,16 +526,16 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5409955841027699</v>
+        <v>0.5312479871175523</v>
       </c>
       <c r="G3" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5396318527410965</v>
+        <v>0.5292943649284356</v>
       </c>
       <c r="I3" t="n">
         <v>100</v>
@@ -559,16 +559,16 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4983464241422075</v>
+        <v>0.5188230348886086</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4959595959595959</v>
+        <v>0.5141558441558441</v>
       </c>
       <c r="I4" t="n">
         <v>100</v>
@@ -592,16 +592,16 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4603026481715007</v>
+        <v>0.49125</v>
       </c>
       <c r="G5" t="n">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4534545454545454</v>
+        <v>0.4882105263157894</v>
       </c>
       <c r="I5" t="n">
         <v>100</v>
@@ -625,16 +625,16 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5004001600640255</v>
+        <v>0.5502</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5</v>
+        <v>0.5500450045004501</v>
       </c>
       <c r="I6" t="n">
         <v>100</v>
@@ -658,16 +658,16 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.49</v>
+        <v>0.54</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4871052631578947</v>
+        <v>0.54</v>
       </c>
       <c r="G7" t="n">
-        <v>0.49</v>
+        <v>0.54</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4825816295392127</v>
+        <v>0.54</v>
       </c>
       <c r="I7" t="n">
         <v>90</v>
@@ -691,16 +691,16 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5008028904054597</v>
+        <v>0.5507211538461538</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4995998399359743</v>
+        <v>0.5498649864986498</v>
       </c>
       <c r="I8" t="n">
         <v>90</v>
@@ -724,16 +724,16 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4784332925336597</v>
+        <v>0.4686201298701299</v>
       </c>
       <c r="G9" t="n">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="H9" t="n">
-        <v>0.477487922705314</v>
+        <v>0.4681358657421364</v>
       </c>
       <c r="I9" t="n">
         <v>90</v>
@@ -757,16 +757,16 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4405138498594942</v>
+        <v>0.4814414414414414</v>
       </c>
       <c r="G10" t="n">
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4395518207282913</v>
+        <v>0.4711363636363636</v>
       </c>
       <c r="I10" t="n">
         <v>90</v>
@@ -790,16 +790,16 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4809696969696969</v>
+        <v>0.4702</v>
       </c>
       <c r="G11" t="n">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="H11" t="n">
-        <v>0.47875</v>
+        <v>0.4700530053005301</v>
       </c>
       <c r="I11" t="n">
         <v>90</v>
@@ -823,16 +823,16 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.51</v>
+        <v>0.47</v>
       </c>
       <c r="F12" t="n">
-        <v>0.510625</v>
+        <v>0.4678735632183909</v>
       </c>
       <c r="G12" t="n">
-        <v>0.51</v>
+        <v>0.47</v>
       </c>
       <c r="H12" t="n">
-        <v>0.5098529852985298</v>
+        <v>0.4666337332392378</v>
       </c>
       <c r="I12" t="n">
         <v>80</v>
@@ -856,16 +856,16 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.54</v>
+        <v>0.57</v>
       </c>
       <c r="F13" t="n">
-        <v>0.542545899632803</v>
+        <v>0.5726136363636364</v>
       </c>
       <c r="G13" t="n">
-        <v>0.54</v>
+        <v>0.57</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5377840224809313</v>
+        <v>0.5684912280701755</v>
       </c>
       <c r="I13" t="n">
         <v>80</v>
@@ -889,16 +889,16 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.44</v>
+        <v>0.49</v>
       </c>
       <c r="F14" t="n">
-        <v>0.4351240016813787</v>
+        <v>0.48775</v>
       </c>
       <c r="G14" t="n">
-        <v>0.44</v>
+        <v>0.49</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4331818181818182</v>
+        <v>0.4848891588217431</v>
       </c>
       <c r="I14" t="n">
         <v>80</v>
@@ -922,16 +922,16 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4405138498594942</v>
+        <v>0.4504807692307692</v>
       </c>
       <c r="G15" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4395518207282913</v>
+        <v>0.4498349834983498</v>
       </c>
       <c r="I15" t="n">
         <v>80</v>
@@ -955,16 +955,16 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="F16" t="n">
-        <v>0.4304326923076923</v>
+        <v>0.4606101967081493</v>
       </c>
       <c r="G16" t="n">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="H16" t="n">
-        <v>0.4298289828982898</v>
+        <v>0.4595678271308523</v>
       </c>
       <c r="I16" t="n">
         <v>80</v>
@@ -988,16 +988,16 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.52</v>
+        <v>0.55</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5196467282215977</v>
+        <v>0.5502</v>
       </c>
       <c r="G17" t="n">
-        <v>0.52</v>
+        <v>0.55</v>
       </c>
       <c r="H17" t="n">
-        <v>0.5196153846153846</v>
+        <v>0.5500450045004501</v>
       </c>
       <c r="I17" t="n">
         <v>70</v>
@@ -1021,16 +1021,16 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
       <c r="F18" t="n">
-        <v>0.543555188094254</v>
+        <v>0.5319318181818182</v>
       </c>
       <c r="G18" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
       <c r="H18" t="n">
-        <v>0.5362962962962964</v>
+        <v>0.5283508771929825</v>
       </c>
       <c r="I18" t="n">
         <v>70</v>
@@ -1054,16 +1054,16 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4365605622157916</v>
+        <v>0.4174051407588739</v>
       </c>
       <c r="G19" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="H19" t="n">
-        <v>0.4354747474747475</v>
+        <v>0.4171980676328502</v>
       </c>
       <c r="I19" t="n">
         <v>70</v>
@@ -1087,16 +1087,16 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="F20" t="n">
-        <v>0.4702</v>
+        <v>0.4607272727272728</v>
       </c>
       <c r="G20" t="n">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="H20" t="n">
-        <v>0.4700530053005301</v>
+        <v>0.4587019230769231</v>
       </c>
       <c r="I20" t="n">
         <v>70</v>
@@ -1120,16 +1120,16 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.41</v>
+        <v>0.47</v>
       </c>
       <c r="F21" t="n">
-        <v>0.4102818035426731</v>
+        <v>0.4709166666666667</v>
       </c>
       <c r="G21" t="n">
-        <v>0.41</v>
+        <v>0.47</v>
       </c>
       <c r="H21" t="n">
-        <v>0.4091142027825043</v>
+        <v>0.464710152233088</v>
       </c>
       <c r="I21" t="n">
         <v>70</v>
@@ -1156,13 +1156,13 @@
         <v>0.53</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5295410628019325</v>
+        <v>0.5319318181818182</v>
       </c>
       <c r="G22" t="n">
         <v>0.53</v>
       </c>
       <c r="H22" t="n">
-        <v>0.5292932330827068</v>
+        <v>0.5283508771929825</v>
       </c>
       <c r="I22" t="n">
         <v>60</v>
@@ -1186,16 +1186,16 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="F23" t="n">
-        <v>0.481322860686234</v>
+        <v>0.5008028904054597</v>
       </c>
       <c r="G23" t="n">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="H23" t="n">
-        <v>0.4758132045088567</v>
+        <v>0.4995998399359743</v>
       </c>
       <c r="I23" t="n">
         <v>60</v>
@@ -1219,16 +1219,16 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0.39</v>
+        <v>0.44</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3860344827586206</v>
+        <v>0.4387070707070707</v>
       </c>
       <c r="G24" t="n">
-        <v>0.39</v>
+        <v>0.44</v>
       </c>
       <c r="H24" t="n">
-        <v>0.3861256175017643</v>
+        <v>0.4386511441188278</v>
       </c>
       <c r="I24" t="n">
         <v>60</v>
@@ -1252,16 +1252,16 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F25" t="n">
-        <v>0.4304428341384863</v>
+        <v>0.4404848484848485</v>
       </c>
       <c r="G25" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="H25" t="n">
-        <v>0.4291442298068261</v>
+        <v>0.4386538461538461</v>
       </c>
       <c r="I25" t="n">
         <v>60</v>
@@ -1285,16 +1285,16 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F26" t="n">
-        <v>0.4404848484848485</v>
+        <v>0.4505681818181818</v>
       </c>
       <c r="G26" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="H26" t="n">
-        <v>0.4386538461538461</v>
+        <v>0.4480701754385965</v>
       </c>
       <c r="I26" t="n">
         <v>60</v>
@@ -1318,16 +1318,16 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="F27" t="n">
-        <v>0.4991919191919192</v>
+        <v>0.4678735632183909</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="H27" t="n">
-        <v>0.4987956643918105</v>
+        <v>0.4666337332392378</v>
       </c>
       <c r="I27" t="n">
         <v>50</v>
@@ -1351,16 +1351,16 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5012121212121212</v>
+        <v>0.4902</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="H28" t="n">
-        <v>0.4987980769230769</v>
+        <v>0.4900510051005101</v>
       </c>
       <c r="I28" t="n">
         <v>50</v>
@@ -1384,16 +1384,16 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.37</v>
+        <v>0.45</v>
       </c>
       <c r="F29" t="n">
-        <v>0.368768115942029</v>
+        <v>0.4474137931034483</v>
       </c>
       <c r="G29" t="n">
-        <v>0.37</v>
+        <v>0.45</v>
       </c>
       <c r="H29" t="n">
-        <v>0.3690526315789474</v>
+        <v>0.4465067043048694</v>
       </c>
       <c r="I29" t="n">
         <v>50</v>
@@ -1417,16 +1417,16 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="F30" t="n">
-        <v>0.4304326923076923</v>
+        <v>0.4504807692307692</v>
       </c>
       <c r="G30" t="n">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="H30" t="n">
-        <v>0.4298289828982898</v>
+        <v>0.4498349834983498</v>
       </c>
       <c r="I30" t="n">
         <v>50</v>
@@ -1453,13 +1453,13 @@
         <v>0.44</v>
       </c>
       <c r="F31" t="n">
-        <v>0.4402611179110567</v>
+        <v>0.4398346424142208</v>
       </c>
       <c r="G31" t="n">
         <v>0.44</v>
       </c>
       <c r="H31" t="n">
-        <v>0.4373022882376556</v>
+        <v>0.4354911433172303</v>
       </c>
       <c r="I31" t="n">
         <v>50</v>
@@ -1483,16 +1483,16 @@
         <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="F32" t="n">
-        <v>0.6109333333333333</v>
+        <v>0.5885714285714286</v>
       </c>
       <c r="G32" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="H32" t="n">
-        <v>0.6093801413509443</v>
+        <v>0.571222729578894</v>
       </c>
       <c r="I32" t="n">
         <v>100</v>
@@ -1516,16 +1516,16 @@
         <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>0.61</v>
+        <v>0.63</v>
       </c>
       <c r="F33" t="n">
-        <v>0.5972043010752688</v>
+        <v>0.6157066537153958</v>
       </c>
       <c r="G33" t="n">
-        <v>0.61</v>
+        <v>0.63</v>
       </c>
       <c r="H33" t="n">
-        <v>0.6006372386325921</v>
+        <v>0.6176680507238246</v>
       </c>
       <c r="I33" t="n">
         <v>100</v>
@@ -1549,16 +1549,16 @@
         <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="F34" t="n">
-        <v>0.6094117647058824</v>
+        <v>0.6157066537153958</v>
       </c>
       <c r="G34" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="H34" t="n">
-        <v>0.6124835164835164</v>
+        <v>0.6176680507238246</v>
       </c>
       <c r="I34" t="n">
         <v>100</v>
@@ -1582,16 +1582,16 @@
         <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6351086956521739</v>
+        <v>0.6724444444444444</v>
       </c>
       <c r="G35" t="n">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="H35" t="n">
-        <v>0.557673630717109</v>
+        <v>0.5921491228070175</v>
       </c>
       <c r="I35" t="n">
         <v>100</v>
@@ -1615,16 +1615,16 @@
         <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="F36" t="n">
-        <v>0.6235343035343035</v>
+        <v>0.6042637362637362</v>
       </c>
       <c r="G36" t="n">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="H36" t="n">
-        <v>0.6221323529411765</v>
+        <v>0.6065926005824614</v>
       </c>
       <c r="I36" t="n">
         <v>100</v>
@@ -1648,16 +1648,16 @@
         <v>1</v>
       </c>
       <c r="E37" t="n">
-        <v>0.63</v>
+        <v>0.68</v>
       </c>
       <c r="F37" t="n">
-        <v>0.6071488848704039</v>
+        <v>0.6698684210526316</v>
       </c>
       <c r="G37" t="n">
-        <v>0.63</v>
+        <v>0.68</v>
       </c>
       <c r="H37" t="n">
-        <v>0.5989998797932443</v>
+        <v>0.6601028517999065</v>
       </c>
       <c r="I37" t="n">
         <v>90</v>
@@ -1681,16 +1681,16 @@
         <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>0.58</v>
+        <v>0.6</v>
       </c>
       <c r="F38" t="n">
-        <v>0.5589682539682539</v>
+        <v>0.5811507936507937</v>
       </c>
       <c r="G38" t="n">
-        <v>0.58</v>
+        <v>0.6</v>
       </c>
       <c r="H38" t="n">
-        <v>0.563853459972863</v>
+        <v>0.584622342831298</v>
       </c>
       <c r="I38" t="n">
         <v>90</v>
@@ -1714,16 +1714,16 @@
         <v>1</v>
       </c>
       <c r="E39" t="n">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="F39" t="n">
-        <v>0.5906341958396752</v>
+        <v>0.5680669710806697</v>
       </c>
       <c r="G39" t="n">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="H39" t="n">
-        <v>0.5928888888888889</v>
+        <v>0.5720113960113961</v>
       </c>
       <c r="I39" t="n">
         <v>90</v>
@@ -1747,16 +1747,16 @@
         <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>0.61</v>
+        <v>0.63</v>
       </c>
       <c r="F40" t="n">
-        <v>0.5628396322778345</v>
+        <v>0.6062759462759462</v>
       </c>
       <c r="G40" t="n">
-        <v>0.61</v>
+        <v>0.63</v>
       </c>
       <c r="H40" t="n">
-        <v>0.5374185700770374</v>
+        <v>0.5509164233069114</v>
       </c>
       <c r="I40" t="n">
         <v>90</v>
@@ -1780,16 +1780,16 @@
         <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5972043010752688</v>
+        <v>0.5798914518317503</v>
       </c>
       <c r="G41" t="n">
-        <v>0.61</v>
+        <v>0.59</v>
       </c>
       <c r="H41" t="n">
-        <v>0.6006372386325921</v>
+        <v>0.5835091167157986</v>
       </c>
       <c r="I41" t="n">
         <v>90</v>
@@ -1813,16 +1813,16 @@
         <v>1</v>
       </c>
       <c r="E42" t="n">
-        <v>0.67</v>
+        <v>0.63</v>
       </c>
       <c r="F42" t="n">
-        <v>0.6590355635925256</v>
+        <v>0.6071488848704039</v>
       </c>
       <c r="G42" t="n">
-        <v>0.67</v>
+        <v>0.63</v>
       </c>
       <c r="H42" t="n">
-        <v>0.6423512441399207</v>
+        <v>0.5989998797932443</v>
       </c>
       <c r="I42" t="n">
         <v>80</v>
@@ -1849,13 +1849,13 @@
         <v>0.61</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5874666666666667</v>
+        <v>0.5972043010752688</v>
       </c>
       <c r="G43" t="n">
         <v>0.61</v>
       </c>
       <c r="H43" t="n">
-        <v>0.5882655543969413</v>
+        <v>0.6006372386325921</v>
       </c>
       <c r="I43" t="n">
         <v>80</v>
@@ -1879,16 +1879,16 @@
         <v>1</v>
       </c>
       <c r="E44" t="n">
-        <v>0.6</v>
+        <v>0.58</v>
       </c>
       <c r="F44" t="n">
-        <v>0.5775467775467775</v>
+        <v>0.5545530145530145</v>
       </c>
       <c r="G44" t="n">
-        <v>0.6</v>
+        <v>0.58</v>
       </c>
       <c r="H44" t="n">
-        <v>0.5801470588235295</v>
+        <v>0.5591544117647058</v>
       </c>
       <c r="I44" t="n">
         <v>80</v>
@@ -1912,16 +1912,16 @@
         <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5845454545454545</v>
+        <v>0.6062759462759462</v>
       </c>
       <c r="G45" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="H45" t="n">
-        <v>0.5541333333333334</v>
+        <v>0.5509164233069114</v>
       </c>
       <c r="I45" t="n">
         <v>80</v>
@@ -1945,16 +1945,16 @@
         <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>0.57</v>
+        <v>0.61</v>
       </c>
       <c r="F46" t="n">
-        <v>0.5591225689733151</v>
+        <v>0.6006603346901855</v>
       </c>
       <c r="G46" t="n">
-        <v>0.57</v>
+        <v>0.61</v>
       </c>
       <c r="H46" t="n">
-        <v>0.5631924882629107</v>
+        <v>0.6038257451686866</v>
       </c>
       <c r="I46" t="n">
         <v>80</v>
@@ -1978,16 +1978,16 @@
         <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>0.61</v>
+        <v>0.65</v>
       </c>
       <c r="F47" t="n">
-        <v>0.5780246913580247</v>
+        <v>0.6330922242314646</v>
       </c>
       <c r="G47" t="n">
-        <v>0.61</v>
+        <v>0.65</v>
       </c>
       <c r="H47" t="n">
-        <v>0.5709090909090909</v>
+        <v>0.6206755619665825</v>
       </c>
       <c r="I47" t="n">
         <v>70</v>
@@ -2011,16 +2011,16 @@
         <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
       <c r="F48" t="n">
-        <v>0.6157066537153958</v>
+        <v>0.5938708110733366</v>
       </c>
       <c r="G48" t="n">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
       <c r="H48" t="n">
-        <v>0.6176680507238246</v>
+        <v>0.5970014588710582</v>
       </c>
       <c r="I48" t="n">
         <v>70</v>
@@ -2044,16 +2044,16 @@
         <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>0.55</v>
+        <v>0.57</v>
       </c>
       <c r="F49" t="n">
-        <v>0.5170666666666667</v>
+        <v>0.5501991257892181</v>
       </c>
       <c r="G49" t="n">
-        <v>0.55</v>
+        <v>0.57</v>
       </c>
       <c r="H49" t="n">
-        <v>0.5249217935349322</v>
+        <v>0.5556682751655257</v>
       </c>
       <c r="I49" t="n">
         <v>70</v>
@@ -2077,16 +2077,16 @@
         <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="F50" t="n">
-        <v>0.5628396322778345</v>
+        <v>0.5885714285714286</v>
       </c>
       <c r="G50" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="H50" t="n">
-        <v>0.5374185700770374</v>
+        <v>0.571222729578894</v>
       </c>
       <c r="I50" t="n">
         <v>70</v>
@@ -2113,13 +2113,13 @@
         <v>0.57</v>
       </c>
       <c r="F51" t="n">
-        <v>0.5501991257892181</v>
+        <v>0.5634725274725274</v>
       </c>
       <c r="G51" t="n">
         <v>0.57</v>
       </c>
       <c r="H51" t="n">
-        <v>0.5556682751655257</v>
+        <v>0.5662431237191242</v>
       </c>
       <c r="I51" t="n">
         <v>70</v>
@@ -2146,13 +2146,13 @@
         <v>0.59</v>
       </c>
       <c r="F52" t="n">
-        <v>0.5639999999999999</v>
+        <v>0.5597628458498023</v>
       </c>
       <c r="G52" t="n">
         <v>0.59</v>
       </c>
       <c r="H52" t="n">
-        <v>0.5671509674429384</v>
+        <v>0.5617124660926995</v>
       </c>
       <c r="I52" t="n">
         <v>60</v>
@@ -2176,16 +2176,16 @@
         <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="F53" t="n">
-        <v>0.6062857142857143</v>
+        <v>0.5938708110733366</v>
       </c>
       <c r="G53" t="n">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="H53" t="n">
-        <v>0.609162210338681</v>
+        <v>0.5970014588710582</v>
       </c>
       <c r="I53" t="n">
         <v>60</v>
@@ -2209,16 +2209,16 @@
         <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="F54" t="n">
-        <v>0.56625</v>
+        <v>0.5680669710806697</v>
       </c>
       <c r="G54" t="n">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="H54" t="n">
-        <v>0.563283147158815</v>
+        <v>0.5720113960113961</v>
       </c>
       <c r="I54" t="n">
         <v>60</v>
@@ -2242,16 +2242,16 @@
         <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="F55" t="n">
-        <v>0.6232575757575758</v>
+        <v>0.5673386383731212</v>
       </c>
       <c r="G55" t="n">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="H55" t="n">
-        <v>0.5776</v>
+        <v>0.5471298855112515</v>
       </c>
       <c r="I55" t="n">
         <v>60</v>
@@ -2275,16 +2275,16 @@
         <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="F56" t="n">
-        <v>0.5510160427807487</v>
+        <v>0.6476984126984127</v>
       </c>
       <c r="G56" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="H56" t="n">
-        <v>0.5546527777777778</v>
+        <v>0.6469289914066034</v>
       </c>
       <c r="I56" t="n">
         <v>60</v>
@@ -2308,16 +2308,16 @@
         <v>1</v>
       </c>
       <c r="E57" t="n">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="F57" t="n">
-        <v>0.6458771929824562</v>
+        <v>0.6071488848704039</v>
       </c>
       <c r="G57" t="n">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="H57" t="n">
-        <v>0.6388592800374007</v>
+        <v>0.5989998797932443</v>
       </c>
       <c r="I57" t="n">
         <v>50</v>
@@ -2341,16 +2341,16 @@
         <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
       <c r="F58" t="n">
-        <v>0.6157066537153958</v>
+        <v>0.5847619047619047</v>
       </c>
       <c r="G58" t="n">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
       <c r="H58" t="n">
-        <v>0.6176680507238246</v>
+        <v>0.5885918003565063</v>
       </c>
       <c r="I58" t="n">
         <v>50</v>
@@ -2374,16 +2374,16 @@
         <v>1</v>
       </c>
       <c r="E59" t="n">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
       <c r="F59" t="n">
-        <v>0.5499122807017544</v>
+        <v>0.5597628458498023</v>
       </c>
       <c r="G59" t="n">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
       <c r="H59" t="n">
-        <v>0.5538849929873773</v>
+        <v>0.5617124660926995</v>
       </c>
       <c r="I59" t="n">
         <v>50</v>
@@ -2407,16 +2407,16 @@
         <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>0.62</v>
+        <v>0.6</v>
       </c>
       <c r="F60" t="n">
-        <v>0.5885714285714286</v>
+        <v>0.5458333333333334</v>
       </c>
       <c r="G60" t="n">
-        <v>0.62</v>
+        <v>0.6</v>
       </c>
       <c r="H60" t="n">
-        <v>0.571222729578894</v>
+        <v>0.5306666666666666</v>
       </c>
       <c r="I60" t="n">
         <v>50</v>
@@ -2440,16 +2440,16 @@
         <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>0.61</v>
+        <v>0.68</v>
       </c>
       <c r="F61" t="n">
-        <v>0.5874666666666667</v>
+        <v>0.672389705882353</v>
       </c>
       <c r="G61" t="n">
-        <v>0.61</v>
+        <v>0.68</v>
       </c>
       <c r="H61" t="n">
-        <v>0.5882655543969413</v>
+        <v>0.6736703296703297</v>
       </c>
       <c r="I61" t="n">
         <v>50</v>
@@ -2473,16 +2473,16 @@
         <v>2</v>
       </c>
       <c r="E62" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F62" t="n">
-        <v>0.5345652173913044</v>
+        <v>0.5624969987995198</v>
       </c>
       <c r="G62" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H62" t="n">
-        <v>0.5296709670967097</v>
+        <v>0.5603521408563426</v>
       </c>
       <c r="I62" t="n">
         <v>100</v>
@@ -2506,16 +2506,16 @@
         <v>2</v>
       </c>
       <c r="E63" t="n">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="F63" t="n">
-        <v>0.6064646464646465</v>
+        <v>0.5918000000000001</v>
       </c>
       <c r="G63" t="n">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="H63" t="n">
-        <v>0.599359743897559</v>
+        <v>0.5903693323991592</v>
       </c>
       <c r="I63" t="n">
         <v>100</v>
@@ -2542,13 +2542,13 @@
         <v>0.59</v>
       </c>
       <c r="F64" t="n">
-        <v>0.5952415458937197</v>
+        <v>0.5918000000000001</v>
       </c>
       <c r="G64" t="n">
         <v>0.59</v>
       </c>
       <c r="H64" t="n">
-        <v>0.5897129712971297</v>
+        <v>0.5903693323991592</v>
       </c>
       <c r="I64" t="n">
         <v>100</v>
@@ -2572,16 +2572,16 @@
         <v>2</v>
       </c>
       <c r="E65" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="F65" t="n">
-        <v>0.608727422003284</v>
+        <v>0.6193947036569988</v>
       </c>
       <c r="G65" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="H65" t="n">
-        <v>0.6078287276040085</v>
+        <v>0.6156589147286822</v>
       </c>
       <c r="I65" t="n">
         <v>100</v>
@@ -2605,16 +2605,16 @@
         <v>2</v>
       </c>
       <c r="E66" t="n">
-        <v>0.57</v>
+        <v>0.58</v>
       </c>
       <c r="F66" t="n">
-        <v>0.5819166666666666</v>
+        <v>0.5884047327621379</v>
       </c>
       <c r="G66" t="n">
-        <v>0.57</v>
+        <v>0.58</v>
       </c>
       <c r="H66" t="n">
-        <v>0.5660677318862426</v>
+        <v>0.5783173076923077</v>
       </c>
       <c r="I66" t="n">
         <v>100</v>
@@ -2638,16 +2638,16 @@
         <v>2</v>
       </c>
       <c r="E67" t="n">
-        <v>0.55</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F67" t="n">
-        <v>0.5585796387520525</v>
+        <v>0.5624969987995198</v>
       </c>
       <c r="G67" t="n">
-        <v>0.55</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H67" t="n">
-        <v>0.5475187969924812</v>
+        <v>0.5603521408563426</v>
       </c>
       <c r="I67" t="n">
         <v>90</v>
@@ -2671,16 +2671,16 @@
         <v>2</v>
       </c>
       <c r="E68" t="n">
-        <v>0.55</v>
+        <v>0.61</v>
       </c>
       <c r="F68" t="n">
-        <v>0.5505608974358974</v>
+        <v>0.6118</v>
       </c>
       <c r="G68" t="n">
-        <v>0.55</v>
+        <v>0.61</v>
       </c>
       <c r="H68" t="n">
-        <v>0.5502255639097744</v>
+        <v>0.6103513161845661</v>
       </c>
       <c r="I68" t="n">
         <v>90</v>
@@ -2704,16 +2704,16 @@
         <v>2</v>
       </c>
       <c r="E69" t="n">
-        <v>0.53</v>
+        <v>0.55</v>
       </c>
       <c r="F69" t="n">
-        <v>0.5345652173913044</v>
+        <v>0.5585796387520525</v>
       </c>
       <c r="G69" t="n">
-        <v>0.53</v>
+        <v>0.55</v>
       </c>
       <c r="H69" t="n">
-        <v>0.5296709670967097</v>
+        <v>0.5475187969924812</v>
       </c>
       <c r="I69" t="n">
         <v>90</v>
@@ -2737,16 +2737,16 @@
         <v>2</v>
       </c>
       <c r="E70" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="F70" t="n">
-        <v>0.6088333333333334</v>
+        <v>0.6193947036569988</v>
       </c>
       <c r="G70" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="H70" t="n">
-        <v>0.6063899908452853</v>
+        <v>0.6156589147286822</v>
       </c>
       <c r="I70" t="n">
         <v>90</v>
@@ -2773,13 +2773,13 @@
         <v>0.55</v>
       </c>
       <c r="F71" t="n">
-        <v>0.5608333333333333</v>
+        <v>0.5565746753246753</v>
       </c>
       <c r="G71" t="n">
         <v>0.55</v>
       </c>
       <c r="H71" t="n">
-        <v>0.5458848356949051</v>
+        <v>0.5487839055149635</v>
       </c>
       <c r="I71" t="n">
         <v>90</v>
@@ -2803,16 +2803,16 @@
         <v>2</v>
       </c>
       <c r="E72" t="n">
-        <v>0.58</v>
+        <v>0.52</v>
       </c>
       <c r="F72" t="n">
-        <v>0.5861414141414142</v>
+        <v>0.5266911464708283</v>
       </c>
       <c r="G72" t="n">
-        <v>0.58</v>
+        <v>0.52</v>
       </c>
       <c r="H72" t="n">
-        <v>0.579327731092437</v>
+        <v>0.5180769230769231</v>
       </c>
       <c r="I72" t="n">
         <v>80</v>
@@ -2836,16 +2836,16 @@
         <v>2</v>
       </c>
       <c r="E73" t="n">
-        <v>0.6</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F73" t="n">
-        <v>0.6</v>
+        <v>0.5624969987995198</v>
       </c>
       <c r="G73" t="n">
-        <v>0.6</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H73" t="n">
-        <v>0.6</v>
+        <v>0.5603521408563426</v>
       </c>
       <c r="I73" t="n">
         <v>80</v>
@@ -2869,16 +2869,16 @@
         <v>2</v>
       </c>
       <c r="E74" t="n">
-        <v>0.52</v>
+        <v>0.58</v>
       </c>
       <c r="F74" t="n">
-        <v>0.5224329731892756</v>
+        <v>0.5825290116046419</v>
       </c>
       <c r="G74" t="n">
-        <v>0.52</v>
+        <v>0.58</v>
       </c>
       <c r="H74" t="n">
-        <v>0.5203841536614646</v>
+        <v>0.5803361344537815</v>
       </c>
       <c r="I74" t="n">
         <v>80</v>
@@ -2902,16 +2902,16 @@
         <v>2</v>
       </c>
       <c r="E75" t="n">
-        <v>0.6</v>
+        <v>0.66</v>
       </c>
       <c r="F75" t="n">
-        <v>0.5985117817279868</v>
+        <v>0.6715194015895278</v>
       </c>
       <c r="G75" t="n">
-        <v>0.6</v>
+        <v>0.66</v>
       </c>
       <c r="H75" t="n">
-        <v>0.5970779220779221</v>
+        <v>0.6474232870954182</v>
       </c>
       <c r="I75" t="n">
         <v>80</v>
@@ -2938,13 +2938,13 @@
         <v>0.5</v>
       </c>
       <c r="F76" t="n">
-        <v>0.5074410913600661</v>
+        <v>0.5061199510403916</v>
       </c>
       <c r="G76" t="n">
         <v>0.5</v>
       </c>
       <c r="H76" t="n">
-        <v>0.4963869931754316</v>
+        <v>0.4979967948717949</v>
       </c>
       <c r="I76" t="n">
         <v>80</v>
@@ -2968,16 +2968,16 @@
         <v>2</v>
       </c>
       <c r="E77" t="n">
-        <v>0.57</v>
+        <v>0.54</v>
       </c>
       <c r="F77" t="n">
-        <v>0.5732852564102564</v>
+        <v>0.54</v>
       </c>
       <c r="G77" t="n">
-        <v>0.57</v>
+        <v>0.54</v>
       </c>
       <c r="H77" t="n">
-        <v>0.5702150215021501</v>
+        <v>0.54</v>
       </c>
       <c r="I77" t="n">
         <v>70</v>
@@ -3001,16 +3001,16 @@
         <v>2</v>
       </c>
       <c r="E78" t="n">
-        <v>0.59</v>
+        <v>0.55</v>
       </c>
       <c r="F78" t="n">
-        <v>0.5905288461538462</v>
+        <v>0.5518</v>
       </c>
       <c r="G78" t="n">
-        <v>0.59</v>
+        <v>0.55</v>
       </c>
       <c r="H78" t="n">
-        <v>0.5902055137844612</v>
+        <v>0.5504053648283456</v>
       </c>
       <c r="I78" t="n">
         <v>70</v>
@@ -3034,16 +3034,16 @@
         <v>2</v>
       </c>
       <c r="E79" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.62</v>
       </c>
       <c r="F79" t="n">
-        <v>0.5590303030303031</v>
+        <v>0.6225930372148859</v>
       </c>
       <c r="G79" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.62</v>
       </c>
       <c r="H79" t="n">
-        <v>0.5592914653784219</v>
+        <v>0.6203041216486596</v>
       </c>
       <c r="I79" t="n">
         <v>70</v>
@@ -3067,16 +3067,16 @@
         <v>2</v>
       </c>
       <c r="E80" t="n">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="F80" t="n">
-        <v>0.5986944104447164</v>
+        <v>0.6202574002574002</v>
       </c>
       <c r="G80" t="n">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="H80" t="n">
-        <v>0.5983838383838384</v>
+        <v>0.61376026272578</v>
       </c>
       <c r="I80" t="n">
         <v>70</v>
@@ -3100,16 +3100,16 @@
         <v>2</v>
       </c>
       <c r="E81" t="n">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="F81" t="n">
-        <v>0.5171346469622332</v>
+        <v>0.5237575270975512</v>
       </c>
       <c r="G81" t="n">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="H81" t="n">
-        <v>0.507298245614035</v>
+        <v>0.52</v>
       </c>
       <c r="I81" t="n">
         <v>70</v>
@@ -3133,16 +3133,16 @@
         <v>2</v>
       </c>
       <c r="E82" t="n">
-        <v>0.55</v>
+        <v>0.58</v>
       </c>
       <c r="F82" t="n">
-        <v>0.5565746753246753</v>
+        <v>0.5841910879164993</v>
       </c>
       <c r="G82" t="n">
-        <v>0.55</v>
+        <v>0.58</v>
       </c>
       <c r="H82" t="n">
-        <v>0.5487839055149635</v>
+        <v>0.58</v>
       </c>
       <c r="I82" t="n">
         <v>60</v>
@@ -3166,16 +3166,16 @@
         <v>2</v>
       </c>
       <c r="E83" t="n">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="F83" t="n">
-        <v>0.5547906602254429</v>
+        <v>0.5424649859943977</v>
       </c>
       <c r="G83" t="n">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="H83" t="n">
-        <v>0.5496849684968497</v>
+        <v>0.5403681472589037</v>
       </c>
       <c r="I83" t="n">
         <v>60</v>
@@ -3199,16 +3199,16 @@
         <v>2</v>
       </c>
       <c r="E84" t="n">
-        <v>0.49</v>
+        <v>0.58</v>
       </c>
       <c r="F84" t="n">
-        <v>0.4881006493506493</v>
+        <v>0.58</v>
       </c>
       <c r="G84" t="n">
-        <v>0.49</v>
+        <v>0.58</v>
       </c>
       <c r="H84" t="n">
-        <v>0.4886117552172598</v>
+        <v>0.58</v>
       </c>
       <c r="I84" t="n">
         <v>60</v>
@@ -3232,16 +3232,16 @@
         <v>2</v>
       </c>
       <c r="E85" t="n">
-        <v>0.58</v>
+        <v>0.62</v>
       </c>
       <c r="F85" t="n">
-        <v>0.5784659322725418</v>
+        <v>0.6234192672998643</v>
       </c>
       <c r="G85" t="n">
-        <v>0.58</v>
+        <v>0.62</v>
       </c>
       <c r="H85" t="n">
-        <v>0.5783030303030303</v>
+        <v>0.6089166666666667</v>
       </c>
       <c r="I85" t="n">
         <v>60</v>
@@ -3265,16 +3265,16 @@
         <v>2</v>
       </c>
       <c r="E86" t="n">
-        <v>0.55</v>
+        <v>0.47</v>
       </c>
       <c r="F86" t="n">
-        <v>0.5633701188455009</v>
+        <v>0.4756896551724138</v>
       </c>
       <c r="G86" t="n">
-        <v>0.55</v>
+        <v>0.47</v>
       </c>
       <c r="H86" t="n">
-        <v>0.5438753906643815</v>
+        <v>0.467077694235589</v>
       </c>
       <c r="I86" t="n">
         <v>60</v>
@@ -3298,16 +3298,16 @@
         <v>2</v>
       </c>
       <c r="E87" t="n">
-        <v>0.55</v>
+        <v>0.58</v>
       </c>
       <c r="F87" t="n">
-        <v>0.5532051282051282</v>
+        <v>0.5841910879164993</v>
       </c>
       <c r="G87" t="n">
-        <v>0.55</v>
+        <v>0.58</v>
       </c>
       <c r="H87" t="n">
-        <v>0.5502250225022501</v>
+        <v>0.58</v>
       </c>
       <c r="I87" t="n">
         <v>50</v>
@@ -3331,16 +3331,16 @@
         <v>2</v>
       </c>
       <c r="E88" t="n">
-        <v>0.57</v>
+        <v>0.59</v>
       </c>
       <c r="F88" t="n">
-        <v>0.5695088566827696</v>
+        <v>0.5933653846153847</v>
       </c>
       <c r="G88" t="n">
-        <v>0.57</v>
+        <v>0.59</v>
       </c>
       <c r="H88" t="n">
-        <v>0.5696975178374032</v>
+        <v>0.5902050205020503</v>
       </c>
       <c r="I88" t="n">
         <v>50</v>
@@ -3364,16 +3364,16 @@
         <v>2</v>
       </c>
       <c r="E89" t="n">
-        <v>0.51</v>
+        <v>0.62</v>
       </c>
       <c r="F89" t="n">
-        <v>0.5070853858784893</v>
+        <v>0.6193947036569988</v>
       </c>
       <c r="G89" t="n">
-        <v>0.51</v>
+        <v>0.62</v>
       </c>
       <c r="H89" t="n">
-        <v>0.5072719910922158</v>
+        <v>0.6156589147286822</v>
       </c>
       <c r="I89" t="n">
         <v>50</v>
@@ -3397,16 +3397,16 @@
         <v>2</v>
       </c>
       <c r="E90" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.57</v>
       </c>
       <c r="F90" t="n">
-        <v>0.5568351648351648</v>
+        <v>0.580125</v>
       </c>
       <c r="G90" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.57</v>
       </c>
       <c r="H90" t="n">
-        <v>0.5501777594047127</v>
+        <v>0.5270048254965772</v>
       </c>
       <c r="I90" t="n">
         <v>50</v>
@@ -3430,16 +3430,16 @@
         <v>2</v>
       </c>
       <c r="E91" t="n">
-        <v>0.49</v>
+        <v>0.61</v>
       </c>
       <c r="F91" t="n">
-        <v>0.5013458110516935</v>
+        <v>0.6118</v>
       </c>
       <c r="G91" t="n">
-        <v>0.49</v>
+        <v>0.61</v>
       </c>
       <c r="H91" t="n">
-        <v>0.4771864510222764</v>
+        <v>0.6103513161845661</v>
       </c>
       <c r="I91" t="n">
         <v>50</v>
@@ -3496,16 +3496,16 @@
         <v>3</v>
       </c>
       <c r="E93" t="n">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="F93" t="n">
-        <v>0.6969761273209549</v>
+        <v>0.6885714285714286</v>
       </c>
       <c r="G93" t="n">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="H93" t="n">
-        <v>0.6933456051541649</v>
+        <v>0.6925874125874125</v>
       </c>
       <c r="I93" t="n">
         <v>100</v>
@@ -3529,16 +3529,16 @@
         <v>3</v>
       </c>
       <c r="E94" t="n">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="F94" t="n">
-        <v>0.694749744637385</v>
+        <v>0.7120000000000001</v>
       </c>
       <c r="G94" t="n">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="H94" t="n">
-        <v>0.6854085045389394</v>
+        <v>0.6928654970760233</v>
       </c>
       <c r="I94" t="n">
         <v>100</v>
@@ -3595,16 +3595,16 @@
         <v>3</v>
       </c>
       <c r="E96" t="n">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
       <c r="F96" t="n">
-        <v>0.5913725490196079</v>
+        <v>0.6185098039215685</v>
       </c>
       <c r="G96" t="n">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
       <c r="H96" t="n">
-        <v>0.6115834691156866</v>
+        <v>0.633778699451933</v>
       </c>
       <c r="I96" t="n">
         <v>100</v>
@@ -3628,16 +3628,16 @@
         <v>3</v>
       </c>
       <c r="E97" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="F97" t="n">
-        <v>0.7578260869565219</v>
+        <v>0.7326007326007326</v>
       </c>
       <c r="G97" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="H97" t="n">
-        <v>0.7079674796747968</v>
+        <v>0.70038136295805</v>
       </c>
       <c r="I97" t="n">
         <v>90</v>
@@ -3661,16 +3661,16 @@
         <v>3</v>
       </c>
       <c r="E98" t="n">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="F98" t="n">
-        <v>0.6999215686274509</v>
+        <v>0.7146428571428572</v>
       </c>
       <c r="G98" t="n">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="H98" t="n">
-        <v>0.7003643904606726</v>
+        <v>0.7145454545454545</v>
       </c>
       <c r="I98" t="n">
         <v>90</v>
@@ -3760,16 +3760,16 @@
         <v>3</v>
       </c>
       <c r="E101" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="F101" t="n">
-        <v>0.5642352941176472</v>
+        <v>0.5582142857142857</v>
       </c>
       <c r="G101" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="H101" t="n">
-        <v>0.5893882387794401</v>
+        <v>0.5827972027972028</v>
       </c>
       <c r="I101" t="n">
         <v>90</v>
@@ -3793,16 +3793,16 @@
         <v>3</v>
       </c>
       <c r="E102" t="n">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="F102" t="n">
-        <v>0.7771631205673759</v>
+        <v>0.6349473684210527</v>
       </c>
       <c r="G102" t="n">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="H102" t="n">
-        <v>0.6982565556343019</v>
+        <v>0.6289094538196334</v>
       </c>
       <c r="I102" t="n">
         <v>80</v>
@@ -3826,16 +3826,16 @@
         <v>3</v>
       </c>
       <c r="E103" t="n">
-        <v>0.75</v>
+        <v>0.72</v>
       </c>
       <c r="F103" t="n">
-        <v>0.7282941777323799</v>
+        <v>0.68</v>
       </c>
       <c r="G103" t="n">
-        <v>0.75</v>
+        <v>0.72</v>
       </c>
       <c r="H103" t="n">
-        <v>0.7087115782767957</v>
+        <v>0.6779999999999999</v>
       </c>
       <c r="I103" t="n">
         <v>80</v>
@@ -3859,16 +3859,16 @@
         <v>3</v>
       </c>
       <c r="E104" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="F104" t="n">
-        <v>0.7771631205673759</v>
+        <v>0.7419354838709676</v>
       </c>
       <c r="G104" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="H104" t="n">
-        <v>0.6982565556343019</v>
+        <v>0.6909090909090909</v>
       </c>
       <c r="I104" t="n">
         <v>80</v>
@@ -3958,16 +3958,16 @@
         <v>3</v>
       </c>
       <c r="E107" t="n">
-        <v>0.74</v>
+        <v>0.76</v>
       </c>
       <c r="F107" t="n">
-        <v>0.7228368794326241</v>
+        <v>0.7771631205673759</v>
       </c>
       <c r="G107" t="n">
-        <v>0.74</v>
+        <v>0.76</v>
       </c>
       <c r="H107" t="n">
-        <v>0.6731112686038272</v>
+        <v>0.6982565556343019</v>
       </c>
       <c r="I107" t="n">
         <v>70</v>
@@ -3994,13 +3994,13 @@
         <v>0.73</v>
       </c>
       <c r="F108" t="n">
-        <v>0.6969761273209549</v>
+        <v>0.694749744637385</v>
       </c>
       <c r="G108" t="n">
         <v>0.73</v>
       </c>
       <c r="H108" t="n">
-        <v>0.6933456051541649</v>
+        <v>0.6854085045389394</v>
       </c>
       <c r="I108" t="n">
         <v>70</v>
@@ -4027,13 +4027,13 @@
         <v>0.75</v>
       </c>
       <c r="F109" t="n">
-        <v>0.7621052631578948</v>
+        <v>0.7326007326007326</v>
       </c>
       <c r="G109" t="n">
         <v>0.75</v>
       </c>
       <c r="H109" t="n">
-        <v>0.6800943567410633</v>
+        <v>0.70038136295805</v>
       </c>
       <c r="I109" t="n">
         <v>70</v>
@@ -4090,16 +4090,16 @@
         <v>3</v>
       </c>
       <c r="E111" t="n">
-        <v>0.65</v>
+        <v>0.61</v>
       </c>
       <c r="F111" t="n">
-        <v>0.5913725490196079</v>
+        <v>0.5525442948263642</v>
       </c>
       <c r="G111" t="n">
-        <v>0.65</v>
+        <v>0.61</v>
       </c>
       <c r="H111" t="n">
-        <v>0.6115834691156866</v>
+        <v>0.5761720430107526</v>
       </c>
       <c r="I111" t="n">
         <v>70</v>
@@ -4123,16 +4123,16 @@
         <v>3</v>
       </c>
       <c r="E112" t="n">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="F112" t="n">
-        <v>0.7621052631578948</v>
+        <v>0.7228368794326241</v>
       </c>
       <c r="G112" t="n">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="H112" t="n">
-        <v>0.6800943567410633</v>
+        <v>0.6731112686038272</v>
       </c>
       <c r="I112" t="n">
         <v>60</v>
@@ -4156,16 +4156,16 @@
         <v>3</v>
       </c>
       <c r="E113" t="n">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="F113" t="n">
-        <v>0.694749744637385</v>
+        <v>0.6782707299787384</v>
       </c>
       <c r="G113" t="n">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="H113" t="n">
-        <v>0.6854085045389394</v>
+        <v>0.6848458781362007</v>
       </c>
       <c r="I113" t="n">
         <v>60</v>
@@ -4192,13 +4192,13 @@
         <v>0.75</v>
       </c>
       <c r="F114" t="n">
-        <v>0.8144329896907218</v>
+        <v>0.7419354838709676</v>
       </c>
       <c r="G114" t="n">
         <v>0.75</v>
       </c>
       <c r="H114" t="n">
-        <v>0.6676846726474518</v>
+        <v>0.6909090909090909</v>
       </c>
       <c r="I114" t="n">
         <v>60</v>
@@ -4222,16 +4222,16 @@
         <v>3</v>
       </c>
       <c r="E115" t="n">
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
       <c r="F115" t="n">
-        <v>0.7984</v>
+        <v>0.8036363636363637</v>
       </c>
       <c r="G115" t="n">
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
       <c r="H115" t="n">
-        <v>0.6027906976744186</v>
+        <v>0.6256261343012703</v>
       </c>
       <c r="I115" t="n">
         <v>60</v>
@@ -4255,16 +4255,16 @@
         <v>3</v>
       </c>
       <c r="E116" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="F116" t="n">
-        <v>0.6531254429482637</v>
+        <v>0.5419883040935671</v>
       </c>
       <c r="G116" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="H116" t="n">
-        <v>0.6631111111111112</v>
+        <v>0.5628035043804755</v>
       </c>
       <c r="I116" t="n">
         <v>60</v>
@@ -4291,13 +4291,13 @@
         <v>0.74</v>
       </c>
       <c r="F117" t="n">
-        <v>0.715</v>
+        <v>0.7425</v>
       </c>
       <c r="G117" t="n">
         <v>0.74</v>
       </c>
       <c r="H117" t="n">
-        <v>0.6836314363143632</v>
+        <v>0.6610714285714286</v>
       </c>
       <c r="I117" t="n">
         <v>50</v>
@@ -4321,16 +4321,16 @@
         <v>3</v>
       </c>
       <c r="E118" t="n">
-        <v>0.74</v>
+        <v>0.71</v>
       </c>
       <c r="F118" t="n">
-        <v>0.7115151515151515</v>
+        <v>0.6612053115423902</v>
       </c>
       <c r="G118" t="n">
-        <v>0.74</v>
+        <v>0.71</v>
       </c>
       <c r="H118" t="n">
-        <v>0.7010000000000001</v>
+        <v>0.662105430801083</v>
       </c>
       <c r="I118" t="n">
         <v>50</v>
@@ -4354,16 +4354,16 @@
         <v>3</v>
       </c>
       <c r="E119" t="n">
-        <v>0.75</v>
+        <v>0.77</v>
       </c>
       <c r="F119" t="n">
-        <v>0.7621052631578948</v>
+        <v>0.8256842105263158</v>
       </c>
       <c r="G119" t="n">
-        <v>0.75</v>
+        <v>0.77</v>
       </c>
       <c r="H119" t="n">
-        <v>0.6800943567410633</v>
+        <v>0.7056868082017783</v>
       </c>
       <c r="I119" t="n">
         <v>50</v>
@@ -4387,16 +4387,16 @@
         <v>3</v>
       </c>
       <c r="E120" t="n">
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
       <c r="F120" t="n">
-        <v>0.7984</v>
+        <v>0.8036363636363637</v>
       </c>
       <c r="G120" t="n">
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
       <c r="H120" t="n">
-        <v>0.6027906976744186</v>
+        <v>0.6256261343012703</v>
       </c>
       <c r="I120" t="n">
         <v>50</v>
@@ -4420,16 +4420,16 @@
         <v>3</v>
       </c>
       <c r="E121" t="n">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="F121" t="n">
-        <v>0.5913725490196079</v>
+        <v>0.5582142857142857</v>
       </c>
       <c r="G121" t="n">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="H121" t="n">
-        <v>0.6115834691156866</v>
+        <v>0.5827972027972028</v>
       </c>
       <c r="I121" t="n">
         <v>50</v>
@@ -4453,16 +4453,16 @@
         <v>4</v>
       </c>
       <c r="E122" t="n">
-        <v>0.6</v>
+        <v>0.58</v>
       </c>
       <c r="F122" t="n">
-        <v>0.6058823529411765</v>
+        <v>0.5875396825396826</v>
       </c>
       <c r="G122" t="n">
-        <v>0.6</v>
+        <v>0.58</v>
       </c>
       <c r="H122" t="n">
-        <v>0.5866666666666667</v>
+        <v>0.5586078098471986</v>
       </c>
       <c r="I122" t="n">
         <v>100</v>
@@ -4486,16 +4486,16 @@
         <v>4</v>
       </c>
       <c r="E123" t="n">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="F123" t="n">
-        <v>0.6297551184263348</v>
+        <v>0.6402955665024632</v>
       </c>
       <c r="G123" t="n">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="H123" t="n">
-        <v>0.6298145363408522</v>
+        <v>0.6378181818181818</v>
       </c>
       <c r="I123" t="n">
         <v>100</v>
@@ -4519,16 +4519,16 @@
         <v>4</v>
       </c>
       <c r="E124" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F124" t="n">
-        <v>0.5265857212238951</v>
+        <v>0.5617142857142857</v>
       </c>
       <c r="G124" t="n">
-        <v>0.53</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H124" t="n">
-        <v>0.5083138000211171</v>
+        <v>0.5416897856242119</v>
       </c>
       <c r="I124" t="n">
         <v>100</v>
@@ -4585,16 +4585,16 @@
         <v>4</v>
       </c>
       <c r="E126" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="F126" t="n">
-        <v>0.5920000000000001</v>
+        <v>0.6020833333333333</v>
       </c>
       <c r="G126" t="n">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="H126" t="n">
-        <v>0.580669344042838</v>
+        <v>0.5921182266009852</v>
       </c>
       <c r="I126" t="n">
         <v>100</v>
@@ -4618,16 +4618,16 @@
         <v>4</v>
       </c>
       <c r="E127" t="n">
-        <v>0.58</v>
+        <v>0.6</v>
       </c>
       <c r="F127" t="n">
-        <v>0.5851428571428571</v>
+        <v>0.611904761904762</v>
       </c>
       <c r="G127" t="n">
-        <v>0.58</v>
+        <v>0.6</v>
       </c>
       <c r="H127" t="n">
-        <v>0.5625220680958385</v>
+        <v>0.5796264855687606</v>
       </c>
       <c r="I127" t="n">
         <v>90</v>
@@ -4651,16 +4651,16 @@
         <v>4</v>
       </c>
       <c r="E128" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="F128" t="n">
-        <v>0.6303481392557023</v>
+        <v>0.62</v>
       </c>
       <c r="G128" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="H128" t="n">
-        <v>0.630111099989991</v>
+        <v>0.62</v>
       </c>
       <c r="I128" t="n">
         <v>90</v>
@@ -4684,16 +4684,16 @@
         <v>4</v>
       </c>
       <c r="E129" t="n">
-        <v>0.51</v>
+        <v>0.53</v>
       </c>
       <c r="F129" t="n">
-        <v>0.4969980506822612</v>
+        <v>0.5278842676311031</v>
       </c>
       <c r="G129" t="n">
-        <v>0.51</v>
+        <v>0.53</v>
       </c>
       <c r="H129" t="n">
-        <v>0.4573762765121759</v>
+        <v>0.4864785927646863</v>
       </c>
       <c r="I129" t="n">
         <v>90</v>
@@ -4750,16 +4750,16 @@
         <v>4</v>
       </c>
       <c r="E131" t="n">
-        <v>0.54</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F131" t="n">
-        <v>0.5379411764705883</v>
+        <v>0.5617142857142857</v>
       </c>
       <c r="G131" t="n">
-        <v>0.54</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H131" t="n">
-        <v>0.5246666666666667</v>
+        <v>0.5416897856242119</v>
       </c>
       <c r="I131" t="n">
         <v>90</v>
@@ -4783,16 +4783,16 @@
         <v>4</v>
       </c>
       <c r="E132" t="n">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="F132" t="n">
-        <v>0.6058823529411765</v>
+        <v>0.632</v>
       </c>
       <c r="G132" t="n">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="H132" t="n">
-        <v>0.5866666666666667</v>
+        <v>0.604186633039092</v>
       </c>
       <c r="I132" t="n">
         <v>80</v>
@@ -4816,16 +4816,16 @@
         <v>4</v>
       </c>
       <c r="E133" t="n">
-        <v>0.66</v>
+        <v>0.62</v>
       </c>
       <c r="F133" t="n">
-        <v>0.6597101449275362</v>
+        <v>0.62</v>
       </c>
       <c r="G133" t="n">
-        <v>0.66</v>
+        <v>0.62</v>
       </c>
       <c r="H133" t="n">
-        <v>0.6595905258932155</v>
+        <v>0.62</v>
       </c>
       <c r="I133" t="n">
         <v>80</v>
@@ -4852,13 +4852,13 @@
         <v>0.55</v>
       </c>
       <c r="F134" t="n">
-        <v>0.5530666666666667</v>
+        <v>0.5549407114624505</v>
       </c>
       <c r="G134" t="n">
         <v>0.55</v>
       </c>
       <c r="H134" t="n">
-        <v>0.5198576205371589</v>
+        <v>0.5143792990501147</v>
       </c>
       <c r="I134" t="n">
         <v>80</v>
@@ -4915,16 +4915,16 @@
         <v>4</v>
       </c>
       <c r="E136" t="n">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="F136" t="n">
-        <v>0.503562412342216</v>
+        <v>0.5148571428571429</v>
       </c>
       <c r="G136" t="n">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="H136" t="n">
-        <v>0.491699968615964</v>
+        <v>0.5000252206809584</v>
       </c>
       <c r="I136" t="n">
         <v>80</v>
@@ -4948,16 +4948,16 @@
         <v>4</v>
       </c>
       <c r="E137" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.58</v>
       </c>
       <c r="F137" t="n">
-        <v>0.5591666666666667</v>
+        <v>0.5832352941176471</v>
       </c>
       <c r="G137" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.58</v>
       </c>
       <c r="H137" t="n">
-        <v>0.5513300492610838</v>
+        <v>0.5660000000000001</v>
       </c>
       <c r="I137" t="n">
         <v>70</v>
@@ -4981,16 +4981,16 @@
         <v>4</v>
       </c>
       <c r="E138" t="n">
-        <v>0.62</v>
+        <v>0.64</v>
       </c>
       <c r="F138" t="n">
-        <v>0.6208</v>
+        <v>0.6396457326892109</v>
       </c>
       <c r="G138" t="n">
-        <v>0.62</v>
+        <v>0.64</v>
       </c>
       <c r="H138" t="n">
-        <v>0.6201520608243297</v>
+        <v>0.6395664391810517</v>
       </c>
       <c r="I138" t="n">
         <v>70</v>
@@ -5014,16 +5014,16 @@
         <v>4</v>
       </c>
       <c r="E139" t="n">
-        <v>0.58</v>
+        <v>0.54</v>
       </c>
       <c r="F139" t="n">
-        <v>0.5987878787878788</v>
+        <v>0.5418181818181818</v>
       </c>
       <c r="G139" t="n">
-        <v>0.58</v>
+        <v>0.54</v>
       </c>
       <c r="H139" t="n">
-        <v>0.544</v>
+        <v>0.5005714285714286</v>
       </c>
       <c r="I139" t="n">
         <v>70</v>
@@ -5047,16 +5047,16 @@
         <v>4</v>
       </c>
       <c r="E140" t="n">
-        <v>0.54</v>
+        <v>0.55</v>
       </c>
       <c r="F140" t="n">
-        <v>0.5965957446808511</v>
+        <v>0.6631578947368422</v>
       </c>
       <c r="G140" t="n">
-        <v>0.54</v>
+        <v>0.55</v>
       </c>
       <c r="H140" t="n">
-        <v>0.4272754946727549</v>
+        <v>0.4332691567192915</v>
       </c>
       <c r="I140" t="n">
         <v>70</v>
@@ -5080,16 +5080,16 @@
         <v>4</v>
       </c>
       <c r="E141" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="F141" t="n">
-        <v>0.486842105263158</v>
+        <v>0.514054054054054</v>
       </c>
       <c r="G141" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="H141" t="n">
-        <v>0.4635416666666667</v>
+        <v>0.4905534105534106</v>
       </c>
       <c r="I141" t="n">
         <v>70</v>
@@ -5113,16 +5113,16 @@
         <v>4</v>
       </c>
       <c r="E142" t="n">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="F142" t="n">
-        <v>0.6605156037991858</v>
+        <v>0.6235416666666667</v>
       </c>
       <c r="G142" t="n">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="H142" t="n">
-        <v>0.6396514161220044</v>
+        <v>0.612512315270936</v>
       </c>
       <c r="I142" t="n">
         <v>60</v>
@@ -5146,16 +5146,16 @@
         <v>4</v>
       </c>
       <c r="E143" t="n">
-        <v>0.65</v>
+        <v>0.61</v>
       </c>
       <c r="F143" t="n">
-        <v>0.6503401360544216</v>
+        <v>0.609731031714171</v>
       </c>
       <c r="G143" t="n">
-        <v>0.65</v>
+        <v>0.61</v>
       </c>
       <c r="H143" t="n">
-        <v>0.6501050945851266</v>
+        <v>0.6098045112781955</v>
       </c>
       <c r="I143" t="n">
         <v>60</v>
@@ -5179,16 +5179,16 @@
         <v>4</v>
       </c>
       <c r="E144" t="n">
-        <v>0.57</v>
+        <v>0.52</v>
       </c>
       <c r="F144" t="n">
-        <v>0.5867631103074141</v>
+        <v>0.513</v>
       </c>
       <c r="G144" t="n">
-        <v>0.57</v>
+        <v>0.52</v>
       </c>
       <c r="H144" t="n">
-        <v>0.530182542316628</v>
+        <v>0.4720855614973262</v>
       </c>
       <c r="I144" t="n">
         <v>60</v>
@@ -5212,16 +5212,16 @@
         <v>4</v>
       </c>
       <c r="E145" t="n">
-        <v>0.51</v>
+        <v>0.55</v>
       </c>
       <c r="F145" t="n">
-        <v>0.428041237113402</v>
+        <v>0.6631578947368422</v>
       </c>
       <c r="G145" t="n">
-        <v>0.51</v>
+        <v>0.55</v>
       </c>
       <c r="H145" t="n">
-        <v>0.3678168180023688</v>
+        <v>0.4332691567192915</v>
       </c>
       <c r="I145" t="n">
         <v>60</v>
@@ -5245,16 +5245,16 @@
         <v>4</v>
       </c>
       <c r="E146" t="n">
-        <v>0.46</v>
+        <v>0.5</v>
       </c>
       <c r="F146" t="n">
-        <v>0.4473529411764706</v>
+        <v>0.4914285714285714</v>
       </c>
       <c r="G146" t="n">
-        <v>0.46</v>
+        <v>0.5</v>
       </c>
       <c r="H146" t="n">
-        <v>0.442</v>
+        <v>0.4791929382093316</v>
       </c>
       <c r="I146" t="n">
         <v>60</v>
@@ -5278,16 +5278,16 @@
         <v>4</v>
       </c>
       <c r="E147" t="n">
-        <v>0.57</v>
+        <v>0.6</v>
       </c>
       <c r="F147" t="n">
-        <v>0.5702857142857143</v>
+        <v>0.5995169082125604</v>
       </c>
       <c r="G147" t="n">
-        <v>0.57</v>
+        <v>0.6</v>
       </c>
       <c r="H147" t="n">
-        <v>0.5602141900937082</v>
+        <v>0.5995182657567243</v>
       </c>
       <c r="I147" t="n">
         <v>50</v>
@@ -5311,16 +5311,16 @@
         <v>4</v>
       </c>
       <c r="E148" t="n">
-        <v>0.67</v>
+        <v>0.6</v>
       </c>
       <c r="F148" t="n">
-        <v>0.6698032918506623</v>
+        <v>0.6019230769230769</v>
       </c>
       <c r="G148" t="n">
-        <v>0.67</v>
+        <v>0.6</v>
       </c>
       <c r="H148" t="n">
-        <v>0.6698345864661654</v>
+        <v>0.6</v>
       </c>
       <c r="I148" t="n">
         <v>50</v>
@@ -5344,16 +5344,16 @@
         <v>4</v>
       </c>
       <c r="E149" t="n">
-        <v>0.57</v>
+        <v>0.55</v>
       </c>
       <c r="F149" t="n">
-        <v>0.5867631103074141</v>
+        <v>0.5642806520198441</v>
       </c>
       <c r="G149" t="n">
-        <v>0.57</v>
+        <v>0.55</v>
       </c>
       <c r="H149" t="n">
-        <v>0.530182542316628</v>
+        <v>0.4943589743589743</v>
       </c>
       <c r="I149" t="n">
         <v>50</v>
@@ -5377,16 +5377,16 @@
         <v>4</v>
       </c>
       <c r="E150" t="n">
-        <v>0.5</v>
+        <v>0.54</v>
       </c>
       <c r="F150" t="n">
-        <v>0.3854166666666666</v>
+        <v>0.5965957446808511</v>
       </c>
       <c r="G150" t="n">
-        <v>0.5</v>
+        <v>0.54</v>
       </c>
       <c r="H150" t="n">
-        <v>0.3627858627858628</v>
+        <v>0.4272754946727549</v>
       </c>
       <c r="I150" t="n">
         <v>50</v>
@@ -5410,16 +5410,16 @@
         <v>4</v>
       </c>
       <c r="E151" t="n">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="F151" t="n">
-        <v>0.4497682709447415</v>
+        <v>0.4788343856240894</v>
       </c>
       <c r="G151" t="n">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="H151" t="n">
-        <v>0.445936337329475</v>
+        <v>0.4664681659803611</v>
       </c>
       <c r="I151" t="n">
         <v>50</v>

</xml_diff>